<commit_message>
- Add algorithm. - Add metrics. - Refactor REST API. - Refactor frontend.
</commit_message>
<xml_diff>
--- a/src/main/resources/additions/additionalTrueDefects.xlsx
+++ b/src/main/resources/additions/additionalTrueDefects.xlsx
@@ -16,10 +16,10 @@
     <sheet name="trueDefectsFromDB" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">emeSynonyms!$B$1:$G$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">emeSynonyms!$B$1:$G$136</definedName>
     <definedName name="true_defect_1" localSheetId="1">trueDefectsFromDB!$A$1:$H$36</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="414">
   <si>
     <t>D21</t>
   </si>
@@ -1683,11 +1683,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI135"/>
+  <dimension ref="A1:CI136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6032,7 +6032,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>172</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>172</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>172</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>172</v>
       </c>
@@ -6076,41 +6076,58 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>172</v>
       </c>
       <c r="B133" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="C133" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="D133" t="s">
+        <v>383</v>
+      </c>
+      <c r="E133" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>172</v>
       </c>
       <c r="B134" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C134" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>172</v>
       </c>
       <c r="B135" t="s">
+        <v>37</v>
+      </c>
+      <c r="C135" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>172</v>
+      </c>
+      <c r="B136" t="s">
         <v>355</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>356</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G135"/>
+  <autoFilter ref="B1:G136"/>
   <sortState ref="B2:L135">
     <sortCondition ref="C2:C135"/>
   </sortState>

</xml_diff>